<commit_message>
Split random streams init & bugfixes (v0.7.0)
* User can now seed the random stream that generates the seeds for each individual random stream.
* Fixed various bugs.
* Updated the unit tests due to annoying issue appearing with many savefig calls in a short timespan.
</commit_message>
<xml_diff>
--- a/test/excelrequest/plotRequest.xlsx
+++ b/test/excelrequest/plotRequest.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="218">
   <si>
     <t xml:space="preserve">General simulation parameters</t>
   </si>
@@ -1108,7 +1108,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1352,12 +1352,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="4">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11 B14" type="list">
       <formula1>Misc!$B$1:$B$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9" type="whole">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6" type="whole">
@@ -1720,16 +1720,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11:B19" type="list">
-      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B5" type="list">
       <formula1>Misc!$B$1:$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8" type="whole">
       <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11:B19" type="list">
+      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6" type="none">
@@ -20860,10 +20860,10 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
@@ -20894,7 +20894,7 @@
         <v>208</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20952,9 +20952,11 @@
       <c r="B15" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C15" s="45"/>
+      <c r="C15" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="D15" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E15" s="45" t="s">
         <v>15</v>
@@ -20967,9 +20969,11 @@
       <c r="B16" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C16" s="45"/>
+      <c r="C16" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="D16" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E16" s="45" t="s">
         <v>15</v>
@@ -20982,9 +20986,11 @@
       <c r="B17" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="45"/>
+      <c r="C17" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="D17" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>15</v>
@@ -20997,9 +21003,11 @@
       <c r="B18" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="45"/>
+      <c r="C18" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="D18" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E18" s="45" t="s">
         <v>15</v>
@@ -21008,7 +21016,9 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="12"/>
-      <c r="C19" s="45"/>
+      <c r="C19" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D19" s="45" t="s">
         <v>15</v>
       </c>
@@ -21019,7 +21029,9 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="45"/>
+      <c r="C20" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D20" s="45" t="s">
         <v>15</v>
       </c>
@@ -21030,7 +21042,9 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="12"/>
-      <c r="C21" s="45"/>
+      <c r="C21" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D21" s="45" t="s">
         <v>15</v>
       </c>
@@ -21041,7 +21055,9 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="45"/>
+      <c r="C22" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D22" s="45" t="s">
         <v>15</v>
       </c>
@@ -21052,7 +21068,9 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="12"/>
-      <c r="C23" s="45"/>
+      <c r="C23" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D23" s="45" t="s">
         <v>15</v>
       </c>
@@ -21063,7 +21081,9 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="45"/>
+      <c r="C24" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D24" s="45" t="s">
         <v>15</v>
       </c>
@@ -21074,7 +21094,9 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="45"/>
+      <c r="C25" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D25" s="45" t="s">
         <v>15</v>
       </c>
@@ -21085,7 +21107,9 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="45"/>
+      <c r="C26" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D26" s="45" t="s">
         <v>15</v>
       </c>
@@ -21096,7 +21120,9 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
       <c r="B27" s="12"/>
-      <c r="C27" s="45"/>
+      <c r="C27" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D27" s="45" t="s">
         <v>15</v>
       </c>
@@ -21107,7 +21133,9 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="45"/>
+      <c r="C28" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D28" s="45" t="s">
         <v>15</v>
       </c>
@@ -21118,7 +21146,9 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
       <c r="B29" s="12"/>
-      <c r="C29" s="45"/>
+      <c r="C29" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D29" s="45" t="s">
         <v>15</v>
       </c>
@@ -21129,7 +21159,9 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
       <c r="B30" s="12"/>
-      <c r="C30" s="45"/>
+      <c r="C30" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D30" s="45" t="s">
         <v>15</v>
       </c>
@@ -21140,7 +21172,9 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="45"/>
+      <c r="C31" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D31" s="45" t="s">
         <v>15</v>
       </c>
@@ -21151,7 +21185,9 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
       <c r="B32" s="12"/>
-      <c r="C32" s="45"/>
+      <c r="C32" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D32" s="45" t="s">
         <v>15</v>
       </c>
@@ -21162,7 +21198,9 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
       <c r="B33" s="12"/>
-      <c r="C33" s="45"/>
+      <c r="C33" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D33" s="45" t="s">
         <v>15</v>
       </c>
@@ -21173,7 +21211,9 @@
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="12"/>
-      <c r="C34" s="45"/>
+      <c r="C34" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D34" s="45" t="s">
         <v>15</v>
       </c>
@@ -21184,7 +21224,9 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
       <c r="B35" s="12"/>
-      <c r="C35" s="45"/>
+      <c r="C35" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D35" s="45" t="s">
         <v>15</v>
       </c>
@@ -21195,7 +21237,9 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
       <c r="B36" s="12"/>
-      <c r="C36" s="45"/>
+      <c r="C36" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D36" s="45" t="s">
         <v>15</v>
       </c>
@@ -21206,7 +21250,9 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
       <c r="B37" s="12"/>
-      <c r="C37" s="45"/>
+      <c r="C37" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D37" s="45" t="s">
         <v>15</v>
       </c>
@@ -21217,7 +21263,9 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
       <c r="B38" s="12"/>
-      <c r="C38" s="45"/>
+      <c r="C38" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D38" s="45" t="s">
         <v>15</v>
       </c>
@@ -21228,7 +21276,9 @@
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="18"/>
       <c r="B39" s="12"/>
-      <c r="C39" s="45"/>
+      <c r="C39" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D39" s="45" t="s">
         <v>15</v>
       </c>
@@ -21239,7 +21289,9 @@
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="18"/>
       <c r="B40" s="12"/>
-      <c r="C40" s="45"/>
+      <c r="C40" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D40" s="45" t="s">
         <v>15</v>
       </c>
@@ -21250,7 +21302,9 @@
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="18"/>
       <c r="B41" s="12"/>
-      <c r="C41" s="45"/>
+      <c r="C41" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D41" s="45" t="s">
         <v>15</v>
       </c>
@@ -21261,7 +21315,9 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="18"/>
       <c r="B42" s="12"/>
-      <c r="C42" s="45"/>
+      <c r="C42" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D42" s="45" t="s">
         <v>15</v>
       </c>
@@ -21272,7 +21328,9 @@
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="18"/>
       <c r="B43" s="12"/>
-      <c r="C43" s="45"/>
+      <c r="C43" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D43" s="45" t="s">
         <v>15</v>
       </c>
@@ -21283,7 +21341,9 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="18"/>
       <c r="B44" s="12"/>
-      <c r="C44" s="45"/>
+      <c r="C44" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D44" s="45" t="s">
         <v>15</v>
       </c>
@@ -21294,7 +21354,9 @@
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="18"/>
       <c r="B45" s="12"/>
-      <c r="C45" s="45"/>
+      <c r="C45" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D45" s="45" t="s">
         <v>15</v>
       </c>
@@ -21305,7 +21367,9 @@
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="18"/>
       <c r="B46" s="12"/>
-      <c r="C46" s="45"/>
+      <c r="C46" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D46" s="45" t="s">
         <v>15</v>
       </c>
@@ -21316,7 +21380,9 @@
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="18"/>
       <c r="B47" s="12"/>
-      <c r="C47" s="45"/>
+      <c r="C47" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D47" s="45" t="s">
         <v>15</v>
       </c>
@@ -21327,7 +21393,9 @@
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="18"/>
       <c r="B48" s="12"/>
-      <c r="C48" s="45"/>
+      <c r="C48" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D48" s="45" t="s">
         <v>15</v>
       </c>
@@ -21338,7 +21406,9 @@
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="18"/>
       <c r="B49" s="12"/>
-      <c r="C49" s="45"/>
+      <c r="C49" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D49" s="45" t="s">
         <v>15</v>
       </c>
@@ -21349,7 +21419,9 @@
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="18"/>
       <c r="B50" s="12"/>
-      <c r="C50" s="45"/>
+      <c r="C50" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D50" s="45" t="s">
         <v>15</v>
       </c>
@@ -21360,7 +21432,9 @@
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="18"/>
       <c r="B51" s="12"/>
-      <c r="C51" s="45"/>
+      <c r="C51" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D51" s="45" t="s">
         <v>15</v>
       </c>
@@ -21371,7 +21445,9 @@
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="18"/>
       <c r="B52" s="12"/>
-      <c r="C52" s="45"/>
+      <c r="C52" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D52" s="45" t="s">
         <v>15</v>
       </c>
@@ -21382,7 +21458,9 @@
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="18"/>
       <c r="B53" s="12"/>
-      <c r="C53" s="45"/>
+      <c r="C53" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D53" s="45" t="s">
         <v>15</v>
       </c>
@@ -21393,7 +21471,9 @@
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="18"/>
       <c r="B54" s="12"/>
-      <c r="C54" s="45"/>
+      <c r="C54" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D54" s="45" t="s">
         <v>15</v>
       </c>
@@ -21404,7 +21484,9 @@
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="18"/>
       <c r="B55" s="12"/>
-      <c r="C55" s="45"/>
+      <c r="C55" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D55" s="45" t="s">
         <v>15</v>
       </c>
@@ -21415,7 +21497,9 @@
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="18"/>
       <c r="B56" s="12"/>
-      <c r="C56" s="45"/>
+      <c r="C56" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D56" s="45" t="s">
         <v>15</v>
       </c>
@@ -21426,7 +21510,9 @@
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="18"/>
       <c r="B57" s="12"/>
-      <c r="C57" s="45"/>
+      <c r="C57" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D57" s="45" t="s">
         <v>15</v>
       </c>
@@ -21437,7 +21523,9 @@
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="18"/>
       <c r="B58" s="12"/>
-      <c r="C58" s="45"/>
+      <c r="C58" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D58" s="45" t="s">
         <v>15</v>
       </c>
@@ -21448,7 +21536,9 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="18"/>
       <c r="B59" s="12"/>
-      <c r="C59" s="45"/>
+      <c r="C59" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D59" s="45" t="s">
         <v>15</v>
       </c>
@@ -21459,7 +21549,9 @@
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="18"/>
       <c r="B60" s="12"/>
-      <c r="C60" s="45"/>
+      <c r="C60" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D60" s="45" t="s">
         <v>15</v>
       </c>
@@ -21470,7 +21562,9 @@
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="18"/>
       <c r="B61" s="12"/>
-      <c r="C61" s="45"/>
+      <c r="C61" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D61" s="45" t="s">
         <v>15</v>
       </c>
@@ -21481,7 +21575,9 @@
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="18"/>
       <c r="B62" s="12"/>
-      <c r="C62" s="45"/>
+      <c r="C62" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D62" s="45" t="s">
         <v>15</v>
       </c>
@@ -21492,7 +21588,9 @@
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="18"/>
       <c r="B63" s="12"/>
-      <c r="C63" s="45"/>
+      <c r="C63" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D63" s="45" t="s">
         <v>15</v>
       </c>
@@ -21503,7 +21601,9 @@
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="18"/>
       <c r="B64" s="12"/>
-      <c r="C64" s="45"/>
+      <c r="C64" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="D64" s="45" t="s">
         <v>15</v>
       </c>
@@ -21516,12 +21616,12 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A9:B9"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:B7 C15:E64" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:B7 E15:E64 C19:D64" type="list">
       <formula1>Misc!$B$1:$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -21531,6 +21631,10 @@
     </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B15:B64" type="list">
       <formula1>Misc!$G$1:$G$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C15:D18" type="list">
+      <formula1>Misc!$B$1:$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -21552,10 +21656,10 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
@@ -21621,9 +21725,11 @@
       <c r="D7" s="18" t="n">
         <v>12</v>
       </c>
-      <c r="E7" s="45"/>
+      <c r="E7" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G7" s="45" t="s">
         <v>15</v>
@@ -21638,9 +21744,11 @@
       <c r="D8" s="18" t="n">
         <v>12</v>
       </c>
-      <c r="E8" s="45"/>
+      <c r="E8" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F8" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G8" s="45" t="s">
         <v>15</v>
@@ -21657,9 +21765,11 @@
       <c r="D9" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="E9" s="45"/>
+      <c r="E9" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G9" s="45" t="s">
         <v>15</v>
@@ -21676,9 +21786,11 @@
       <c r="D10" s="18" t="n">
         <v>12</v>
       </c>
-      <c r="E10" s="45"/>
+      <c r="E10" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F10" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G10" s="45" t="s">
         <v>15</v>
@@ -21693,9 +21805,11 @@
       <c r="D11" s="18" t="n">
         <v>12</v>
       </c>
-      <c r="E11" s="45"/>
+      <c r="E11" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F11" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G11" s="45" t="s">
         <v>15</v>
@@ -21714,9 +21828,11 @@
       <c r="D12" s="18" t="n">
         <v>12</v>
       </c>
-      <c r="E12" s="45"/>
+      <c r="E12" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F12" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G12" s="45" t="s">
         <v>15</v>
@@ -21735,9 +21851,11 @@
       <c r="D13" s="18" t="n">
         <v>12</v>
       </c>
-      <c r="E13" s="45"/>
+      <c r="E13" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F13" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G13" s="45" t="s">
         <v>15</v>
@@ -21748,7 +21866,9 @@
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="45"/>
+      <c r="E14" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F14" s="45" t="s">
         <v>15</v>
       </c>
@@ -21761,7 +21881,9 @@
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="18"/>
-      <c r="E15" s="45"/>
+      <c r="E15" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F15" s="45" t="s">
         <v>15</v>
       </c>
@@ -21774,7 +21896,9 @@
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="18"/>
-      <c r="E16" s="45"/>
+      <c r="E16" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F16" s="45" t="s">
         <v>15</v>
       </c>
@@ -21787,7 +21911,9 @@
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="18"/>
-      <c r="E17" s="45"/>
+      <c r="E17" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F17" s="45" t="s">
         <v>15</v>
       </c>
@@ -21800,7 +21926,9 @@
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="45"/>
+      <c r="E18" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F18" s="45" t="s">
         <v>15</v>
       </c>
@@ -21813,7 +21941,9 @@
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="45"/>
+      <c r="E19" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F19" s="45" t="s">
         <v>15</v>
       </c>
@@ -21826,7 +21956,9 @@
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="45"/>
+      <c r="E20" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F20" s="45" t="s">
         <v>15</v>
       </c>
@@ -21839,7 +21971,9 @@
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="18"/>
-      <c r="E21" s="45"/>
+      <c r="E21" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F21" s="45" t="s">
         <v>15</v>
       </c>
@@ -21852,7 +21986,9 @@
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="45"/>
+      <c r="E22" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F22" s="45" t="s">
         <v>15</v>
       </c>
@@ -21865,7 +22001,9 @@
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="45"/>
+      <c r="E23" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F23" s="45" t="s">
         <v>15</v>
       </c>
@@ -21878,7 +22016,9 @@
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="45"/>
+      <c r="E24" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F24" s="45" t="s">
         <v>15</v>
       </c>
@@ -21891,7 +22031,9 @@
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="45"/>
+      <c r="E25" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F25" s="45" t="s">
         <v>15</v>
       </c>
@@ -21904,7 +22046,9 @@
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="45"/>
+      <c r="E26" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F26" s="45" t="s">
         <v>15</v>
       </c>
@@ -21917,7 +22061,9 @@
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="45"/>
+      <c r="E27" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F27" s="45" t="s">
         <v>15</v>
       </c>
@@ -21930,7 +22076,9 @@
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="18"/>
-      <c r="E28" s="45"/>
+      <c r="E28" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F28" s="45" t="s">
         <v>15</v>
       </c>
@@ -21943,7 +22091,9 @@
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="18"/>
-      <c r="E29" s="45"/>
+      <c r="E29" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F29" s="45" t="s">
         <v>15</v>
       </c>
@@ -21956,7 +22106,9 @@
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="18"/>
-      <c r="E30" s="45"/>
+      <c r="E30" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F30" s="45" t="s">
         <v>15</v>
       </c>
@@ -21969,7 +22121,9 @@
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="18"/>
-      <c r="E31" s="45"/>
+      <c r="E31" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F31" s="45" t="s">
         <v>15</v>
       </c>
@@ -21982,7 +22136,9 @@
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="18"/>
-      <c r="E32" s="45"/>
+      <c r="E32" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F32" s="45" t="s">
         <v>15</v>
       </c>
@@ -21995,7 +22151,9 @@
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="18"/>
-      <c r="E33" s="45"/>
+      <c r="E33" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F33" s="45" t="s">
         <v>15</v>
       </c>
@@ -22008,7 +22166,9 @@
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="18"/>
-      <c r="E34" s="45"/>
+      <c r="E34" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F34" s="45" t="s">
         <v>15</v>
       </c>
@@ -22021,7 +22181,9 @@
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="18"/>
-      <c r="E35" s="45"/>
+      <c r="E35" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F35" s="45" t="s">
         <v>15</v>
       </c>
@@ -22034,7 +22196,9 @@
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="18"/>
-      <c r="E36" s="45"/>
+      <c r="E36" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F36" s="45" t="s">
         <v>15</v>
       </c>
@@ -22047,7 +22211,9 @@
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="18"/>
-      <c r="E37" s="45"/>
+      <c r="E37" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F37" s="45" t="s">
         <v>15</v>
       </c>
@@ -22060,7 +22226,9 @@
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="18"/>
-      <c r="E38" s="45"/>
+      <c r="E38" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F38" s="45" t="s">
         <v>15</v>
       </c>
@@ -22073,7 +22241,9 @@
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="18"/>
-      <c r="E39" s="45"/>
+      <c r="E39" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F39" s="45" t="s">
         <v>15</v>
       </c>
@@ -22086,7 +22256,9 @@
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="18"/>
-      <c r="E40" s="45"/>
+      <c r="E40" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F40" s="45" t="s">
         <v>15</v>
       </c>
@@ -22099,7 +22271,9 @@
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="18"/>
-      <c r="E41" s="45"/>
+      <c r="E41" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F41" s="45" t="s">
         <v>15</v>
       </c>
@@ -22112,7 +22286,9 @@
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="45"/>
+      <c r="E42" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F42" s="45" t="s">
         <v>15</v>
       </c>
@@ -22125,7 +22301,9 @@
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="18"/>
-      <c r="E43" s="45"/>
+      <c r="E43" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F43" s="45" t="s">
         <v>15</v>
       </c>
@@ -22138,7 +22316,9 @@
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="18"/>
-      <c r="E44" s="45"/>
+      <c r="E44" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F44" s="45" t="s">
         <v>15</v>
       </c>
@@ -22151,7 +22331,9 @@
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="18"/>
-      <c r="E45" s="45"/>
+      <c r="E45" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F45" s="45" t="s">
         <v>15</v>
       </c>
@@ -22164,7 +22346,9 @@
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="18"/>
-      <c r="E46" s="45"/>
+      <c r="E46" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F46" s="45" t="s">
         <v>15</v>
       </c>
@@ -22177,7 +22361,9 @@
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="18"/>
-      <c r="E47" s="45"/>
+      <c r="E47" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F47" s="45" t="s">
         <v>15</v>
       </c>
@@ -22190,7 +22376,9 @@
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="18"/>
-      <c r="E48" s="45"/>
+      <c r="E48" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F48" s="45" t="s">
         <v>15</v>
       </c>
@@ -22203,7 +22391,9 @@
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="18"/>
-      <c r="E49" s="45"/>
+      <c r="E49" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F49" s="45" t="s">
         <v>15</v>
       </c>
@@ -22216,7 +22406,9 @@
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="18"/>
-      <c r="E50" s="45"/>
+      <c r="E50" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F50" s="45" t="s">
         <v>15</v>
       </c>
@@ -22229,7 +22421,9 @@
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="18"/>
-      <c r="E51" s="45"/>
+      <c r="E51" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F51" s="45" t="s">
         <v>15</v>
       </c>
@@ -22242,7 +22436,9 @@
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="18"/>
-      <c r="E52" s="45"/>
+      <c r="E52" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F52" s="45" t="s">
         <v>15</v>
       </c>
@@ -22255,7 +22451,9 @@
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="18"/>
-      <c r="E53" s="45"/>
+      <c r="E53" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F53" s="45" t="s">
         <v>15</v>
       </c>
@@ -22268,7 +22466,9 @@
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="18"/>
-      <c r="E54" s="45"/>
+      <c r="E54" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F54" s="45" t="s">
         <v>15</v>
       </c>
@@ -22281,7 +22481,9 @@
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="18"/>
-      <c r="E55" s="45"/>
+      <c r="E55" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F55" s="45" t="s">
         <v>15</v>
       </c>
@@ -22294,7 +22496,9 @@
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="18"/>
-      <c r="E56" s="45"/>
+      <c r="E56" s="45" t="s">
+        <v>12</v>
+      </c>
       <c r="F56" s="45" t="s">
         <v>15</v>
       </c>
@@ -22311,12 +22515,16 @@
       <formula>'Output plots (trans)'!$A7="NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:G56" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E14:E56" type="list">
+      <formula1>Misc!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:G13 F14:G56" type="list">
       <formula1>Misc!$B$1:$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -22347,10 +22555,10 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -22413,9 +22621,11 @@
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
-      <c r="E7" s="45"/>
+      <c r="E7" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G7" s="45" t="s">
         <v>15</v>
@@ -22434,9 +22644,11 @@
         <v>202</v>
       </c>
       <c r="D8" s="49"/>
-      <c r="E8" s="45"/>
+      <c r="E8" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F8" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G8" s="45" t="s">
         <v>15</v>
@@ -22453,9 +22665,11 @@
         <v>202</v>
       </c>
       <c r="D9" s="49"/>
-      <c r="E9" s="45"/>
+      <c r="E9" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G9" s="45" t="s">
         <v>15</v>
@@ -22472,9 +22686,11 @@
         <v>202</v>
       </c>
       <c r="D10" s="49"/>
-      <c r="E10" s="45"/>
+      <c r="E10" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F10" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G10" s="45" t="s">
         <v>15</v>
@@ -22491,9 +22707,11 @@
         <v>200</v>
       </c>
       <c r="D11" s="49"/>
-      <c r="E11" s="45"/>
+      <c r="E11" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F11" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G11" s="45" t="s">
         <v>15</v>
@@ -22510,9 +22728,11 @@
         <v>200</v>
       </c>
       <c r="D12" s="49"/>
-      <c r="E12" s="45"/>
+      <c r="E12" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F12" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G12" s="45" t="s">
         <v>15</v>
@@ -22529,9 +22749,11 @@
         <v>200</v>
       </c>
       <c r="D13" s="49"/>
-      <c r="E13" s="45"/>
+      <c r="E13" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F13" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G13" s="45" t="s">
         <v>15</v>
@@ -22548,9 +22770,11 @@
         <v>200</v>
       </c>
       <c r="D14" s="49"/>
-      <c r="E14" s="45"/>
+      <c r="E14" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F14" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G14" s="45" t="s">
         <v>15</v>
@@ -22567,9 +22791,11 @@
         <v>200</v>
       </c>
       <c r="D15" s="49"/>
-      <c r="E15" s="45"/>
+      <c r="E15" s="45" t="s">
+        <v>15</v>
+      </c>
       <c r="F15" s="45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G15" s="45" t="s">
         <v>15</v>

</xml_diff>